<commit_message>
fix CeruleanCave and vc patch
</commit_message>
<xml_diff>
--- a/xlsx/buildingsA.xlsx
+++ b/xlsx/buildingsA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-31140" yWindow="1240" windowWidth="27540" windowHeight="27120" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-31140" yWindow="1240" windowWidth="27540" windowHeight="27120" tabRatio="600" firstSheet="13" activeTab="22" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ViridianForest" sheetId="1" state="visible" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="SilphCo5F" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191028" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -25346,8 +25346,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>